<commit_message>
some saving after a stadem demo
</commit_message>
<xml_diff>
--- a/output/syntheses/LGR_Coho_all_summaries_2024-06-21.xlsx
+++ b/output/syntheses/LGR_Coho_all_summaries_2024-06-21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverFishStatus\output\syntheses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C7EF88-D317-4631-9682-185FA8F10C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CBFCD8-0A19-4C14-A1CF-50FF81FA3D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LGR_Esc" sheetId="1" r:id="rId1"/>
@@ -1081,9 +1081,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -3849,7 +3852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>